<commit_message>
Actualizacion del 25 de mayo de 2023
</commit_message>
<xml_diff>
--- a/Query Base de datos.xlsx
+++ b/Query Base de datos.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\unificacion_proyecto_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2843ED7B-6729-460E-AA5C-6AEA5110498A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD650EF3-9FDD-4C8B-9A03-6C0767ED104E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{2A26BEC3-3C8D-473A-BF84-89C24DF24433}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{2A26BEC3-3C8D-473A-BF84-89C24DF24433}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Query_salas" sheetId="2" r:id="rId2"/>
+    <sheet name="Query_comedores" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="336">
   <si>
     <t>Codigo_producto</t>
   </si>
@@ -808,6 +809,243 @@
   </si>
   <si>
     <t>ELSE precio</t>
+  </si>
+  <si>
+    <t>CREATE TABLE comedores (</t>
+  </si>
+  <si>
+    <t>materiales SET (' Madera ',' Vidrio ',' Metal ') NOT NULL</t>
+  </si>
+  <si>
+    <t>comedores</t>
+  </si>
+  <si>
+    <t>Imagenes/comedores/</t>
+  </si>
+  <si>
+    <t>colores SET (' Natural ',' Wengue ', ' Caoba ') NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Natural , Wengue ,  Caoba</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Madera , Vidrio , Metal </t>
+  </si>
+  <si>
+    <t>$ 2.350.000</t>
+  </si>
+  <si>
+    <t>$ 2.830.000</t>
+  </si>
+  <si>
+    <t>$ 3.330.000</t>
+  </si>
+  <si>
+    <t>comedores1</t>
+  </si>
+  <si>
+    <t>comedores2</t>
+  </si>
+  <si>
+    <t>comedores3</t>
+  </si>
+  <si>
+    <t>comedores4</t>
+  </si>
+  <si>
+    <t>comedores5</t>
+  </si>
+  <si>
+    <t>comedores6</t>
+  </si>
+  <si>
+    <t>comedores7</t>
+  </si>
+  <si>
+    <t>comedores8</t>
+  </si>
+  <si>
+    <t>comedores9</t>
+  </si>
+  <si>
+    <t>comedores10</t>
+  </si>
+  <si>
+    <t>comedores11</t>
+  </si>
+  <si>
+    <t>comedores12</t>
+  </si>
+  <si>
+    <t>comedores13</t>
+  </si>
+  <si>
+    <t>comedores14</t>
+  </si>
+  <si>
+    <t>comedores15</t>
+  </si>
+  <si>
+    <t>$ 2.650.000</t>
+  </si>
+  <si>
+    <t>$ 3.350.000</t>
+  </si>
+  <si>
+    <t>$ 2.240.000</t>
+  </si>
+  <si>
+    <t>$ 2.640.000</t>
+  </si>
+  <si>
+    <t>$ 1.750.000</t>
+  </si>
+  <si>
+    <t>$ 2.040.000</t>
+  </si>
+  <si>
+    <t>$ 3.150.000</t>
+  </si>
+  <si>
+    <t>$ 4.990.000</t>
+  </si>
+  <si>
+    <t>Comedor 6 puestos Valenciano</t>
+  </si>
+  <si>
+    <t>Comedor 6 puestos Alaska</t>
+  </si>
+  <si>
+    <t>Comedor 6 puestos Sevilla</t>
+  </si>
+  <si>
+    <t>Comedor 6 puestos Underground</t>
+  </si>
+  <si>
+    <t>Comedor 4 puestos Marsella</t>
+  </si>
+  <si>
+    <t>Comedor 4 puestos Suburbios</t>
+  </si>
+  <si>
+    <t>Comedor 6 puestos Manchester</t>
+  </si>
+  <si>
+    <t>Comedor 4 puestos Mediterraneo</t>
+  </si>
+  <si>
+    <t>Comedor 4 puestos New York</t>
+  </si>
+  <si>
+    <t>Comedor 4 puestos Simple</t>
+  </si>
+  <si>
+    <t>Comedor 4 puestos Ceniza</t>
+  </si>
+  <si>
+    <t>Comedor 6 puestos Europeo</t>
+  </si>
+  <si>
+    <t>Comedor 8 puestos Industrial</t>
+  </si>
+  <si>
+    <t>Comedor 6 puestos Minimalista</t>
+  </si>
+  <si>
+    <t>Comedor 6 puestos Valenciano plus</t>
+  </si>
+  <si>
+    <t>Imagenes/comedores/comedores1.png</t>
+  </si>
+  <si>
+    <t>Imagenes/comedores/comedores2.png</t>
+  </si>
+  <si>
+    <t>Imagenes/comedores/comedores3.png</t>
+  </si>
+  <si>
+    <t>Imagenes/comedores/comedores4.png</t>
+  </si>
+  <si>
+    <t>Imagenes/comedores/comedores5.png</t>
+  </si>
+  <si>
+    <t>Imagenes/comedores/comedores6.png</t>
+  </si>
+  <si>
+    <t>Imagenes/comedores/comedores7.png</t>
+  </si>
+  <si>
+    <t>Imagenes/comedores/comedores8.png</t>
+  </si>
+  <si>
+    <t>Imagenes/comedores/comedores9.png</t>
+  </si>
+  <si>
+    <t>Imagenes/comedores/comedores10.png</t>
+  </si>
+  <si>
+    <t>Imagenes/comedores/comedores11.png</t>
+  </si>
+  <si>
+    <t>Imagenes/comedores/comedores12.png</t>
+  </si>
+  <si>
+    <t>Imagenes/comedores/comedores13.png</t>
+  </si>
+  <si>
+    <t>Imagenes/comedores/comedores14.png</t>
+  </si>
+  <si>
+    <t>Imagenes/comedores/comedores15.png</t>
+  </si>
+  <si>
+    <t>INSERT INTO comedores (codigo, nombre, descripcion, precio, url_imagen, colores, materiales)</t>
+  </si>
+  <si>
+    <t>('comedores1','Comedor 6 puestos Alaska','N/A','$ 3.330.000','Imagenes/comedores/comedores1.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</t>
+  </si>
+  <si>
+    <t>('comedores2','Comedor 6 puestos Sevilla','N/A','$ 2.830.000','Imagenes/comedores/comedores2.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</t>
+  </si>
+  <si>
+    <t>('comedores3','Comedor 6 puestos Underground','N/A','$ 2.350.000','Imagenes/comedores/comedores3.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</t>
+  </si>
+  <si>
+    <t>('comedores4','Comedor 4 puestos Marsella','N/A','$ 3.550.000','Imagenes/comedores/comedores4.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</t>
+  </si>
+  <si>
+    <t>('comedores5','Comedor 6 puestos Valenciano','N/A','$ 4.250.000','Imagenes/comedores/comedores5.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</t>
+  </si>
+  <si>
+    <t>('comedores6','Comedor 4 puestos Suburbios','N/A','$ 2.650.000','Imagenes/comedores/comedores6.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</t>
+  </si>
+  <si>
+    <t>('comedores7','Comedor 6 puestos Manchester','N/A','$ 3.350.000','Imagenes/comedores/comedores7.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</t>
+  </si>
+  <si>
+    <t>('comedores8','Comedor 4 puestos Mediterraneo','N/A','$ 2.240.000','Imagenes/comedores/comedores8.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</t>
+  </si>
+  <si>
+    <t>('comedores9','Comedor 4 puestos New York','N/A','$ 2.640.000','Imagenes/comedores/comedores9.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</t>
+  </si>
+  <si>
+    <t>('comedores10','Comedor 4 puestos Simple','N/A','$ 1.750.000','Imagenes/comedores/comedores10.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</t>
+  </si>
+  <si>
+    <t>('comedores11','Comedor 4 puestos Ceniza','N/A','$ 2.040.000','Imagenes/comedores/comedores11.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</t>
+  </si>
+  <si>
+    <t>('comedores12','Comedor 6 puestos Europeo','N/A','$ 3.150.000','Imagenes/comedores/comedores12.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</t>
+  </si>
+  <si>
+    <t>('comedores13','Comedor 8 puestos Industrial','N/A','$ 4.990.000','Imagenes/comedores/comedores13.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</t>
+  </si>
+  <si>
+    <t>('comedores14','Comedor 6 puestos Minimalista','N/A','$ 2.750.000','Imagenes/comedores/comedores14.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</t>
+  </si>
+  <si>
+    <t>('comedores15','Comedor 6 puestos Valenciano plus','N/A','$ 4.250.000','Imagenes/comedores/comedores15.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</t>
   </si>
 </sst>
 </file>
@@ -1187,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467A2FFE-2E48-41E5-8C10-D293866D1E4B}">
   <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:A45"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1866,8 +2104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAA30AA2-9880-4D41-820C-F91482830A46}">
   <dimension ref="A1:N104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G11" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21:M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3190,4 +3428,1389 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2239FE3-6675-4F43-8E17-8F9AABEB3097}">
+  <dimension ref="A1:N104"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>260</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="L20" t="s">
+        <v>221</v>
+      </c>
+      <c r="M20" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B21" t="s">
+        <v>291</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="H21" t="s">
+        <v>259</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>108</v>
+      </c>
+      <c r="K21" t="str">
+        <f>$H$19&amp;$H$21&amp;I21&amp;$J$21</f>
+        <v>Imagenes/comedores/comedores1.png</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" ref="L21:L30" si="0">+$H$21&amp;I21</f>
+        <v>comedores1</v>
+      </c>
+      <c r="M21" t="str">
+        <f>+"('"&amp;A21&amp;"'"&amp;$L$20&amp;"'"&amp;B21&amp;"'"&amp;$L$20&amp;"'"&amp;C21&amp;"'"&amp;$L$20&amp;"'"&amp;D21&amp;"'"&amp;$L$20&amp;"'"&amp;E21&amp;"'"&amp;$L$20&amp;"'"&amp;F21&amp;"'"&amp;$L$20&amp;"'"&amp;G21&amp;"'),"</f>
+        <v>('comedores1','Comedor 6 puestos Alaska','N/A','$ 3.330.000','Imagenes/comedores/comedores1.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</v>
+      </c>
+      <c r="N21" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B22" t="s">
+        <v>292</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" ref="K22:K30" si="1">$H$19&amp;$H$21&amp;I22&amp;$J$21</f>
+        <v>Imagenes/comedores/comedores2.png</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="0"/>
+        <v>comedores2</v>
+      </c>
+      <c r="M22" s="1" t="str">
+        <f t="shared" ref="M22:M35" si="2">+"('"&amp;A22&amp;"'"&amp;$L$20&amp;"'"&amp;B22&amp;"'"&amp;$L$20&amp;"'"&amp;C22&amp;"'"&amp;$L$20&amp;"'"&amp;D22&amp;"'"&amp;$L$20&amp;"'"&amp;E22&amp;"'"&amp;$L$20&amp;"'"&amp;F22&amp;"'"&amp;$L$20&amp;"'"&amp;G22&amp;"'),"</f>
+        <v>('comedores2','Comedor 6 puestos Sevilla','N/A','$ 2.830.000','Imagenes/comedores/comedores2.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</v>
+      </c>
+      <c r="N22" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B23" t="s">
+        <v>293</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I23">
+        <v>3</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="1"/>
+        <v>Imagenes/comedores/comedores3.png</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="0"/>
+        <v>comedores3</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="2"/>
+        <v>('comedores3','Comedor 6 puestos Underground','N/A','$ 2.350.000','Imagenes/comedores/comedores3.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</v>
+      </c>
+      <c r="N23" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B24" t="s">
+        <v>294</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I24">
+        <v>4</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="1"/>
+        <v>Imagenes/comedores/comedores4.png</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="0"/>
+        <v>comedores4</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="2"/>
+        <v>('comedores4','Comedor 4 puestos Marsella','N/A','$ 3.550.000','Imagenes/comedores/comedores4.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</v>
+      </c>
+      <c r="N24" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B25" t="s">
+        <v>290</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I25">
+        <v>5</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="1"/>
+        <v>Imagenes/comedores/comedores5.png</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="0"/>
+        <v>comedores5</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="2"/>
+        <v>('comedores5','Comedor 6 puestos Valenciano','N/A','$ 4.250.000','Imagenes/comedores/comedores5.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</v>
+      </c>
+      <c r="N25" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B26" t="s">
+        <v>295</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I26">
+        <v>6</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="1"/>
+        <v>Imagenes/comedores/comedores6.png</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="0"/>
+        <v>comedores6</v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="2"/>
+        <v>('comedores6','Comedor 4 puestos Suburbios','N/A','$ 2.650.000','Imagenes/comedores/comedores6.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</v>
+      </c>
+      <c r="N26" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B27" t="s">
+        <v>296</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I27">
+        <v>7</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="1"/>
+        <v>Imagenes/comedores/comedores7.png</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="0"/>
+        <v>comedores7</v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" si="2"/>
+        <v>('comedores7','Comedor 6 puestos Manchester','N/A','$ 3.350.000','Imagenes/comedores/comedores7.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</v>
+      </c>
+      <c r="N27" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B28" t="s">
+        <v>297</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I28">
+        <v>8</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="1"/>
+        <v>Imagenes/comedores/comedores8.png</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="0"/>
+        <v>comedores8</v>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" si="2"/>
+        <v>('comedores8','Comedor 4 puestos Mediterraneo','N/A','$ 2.240.000','Imagenes/comedores/comedores8.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</v>
+      </c>
+      <c r="N28" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="B29" t="s">
+        <v>298</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I29">
+        <v>9</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="1"/>
+        <v>Imagenes/comedores/comedores9.png</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="0"/>
+        <v>comedores9</v>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" si="2"/>
+        <v>('comedores9','Comedor 4 puestos New York','N/A','$ 2.640.000','Imagenes/comedores/comedores9.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</v>
+      </c>
+      <c r="N29" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B30" t="s">
+        <v>299</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I30">
+        <v>10</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="1"/>
+        <v>Imagenes/comedores/comedores10.png</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="0"/>
+        <v>comedores10</v>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" si="2"/>
+        <v>('comedores10','Comedor 4 puestos Simple','N/A','$ 1.750.000','Imagenes/comedores/comedores10.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</v>
+      </c>
+      <c r="N30" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B31" t="s">
+        <v>300</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I31">
+        <v>11</v>
+      </c>
+      <c r="K31" t="str">
+        <f>$H$19&amp;$H$21&amp;I31&amp;$J$21</f>
+        <v>Imagenes/comedores/comedores11.png</v>
+      </c>
+      <c r="L31" t="str">
+        <f>+$H$21&amp;I31</f>
+        <v>comedores11</v>
+      </c>
+      <c r="M31" t="str">
+        <f t="shared" si="2"/>
+        <v>('comedores11','Comedor 4 puestos Ceniza','N/A','$ 2.040.000','Imagenes/comedores/comedores11.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</v>
+      </c>
+      <c r="N31" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B32" t="s">
+        <v>301</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I32">
+        <v>12</v>
+      </c>
+      <c r="K32" t="str">
+        <f>$H$19&amp;$H$21&amp;I32&amp;$J$21</f>
+        <v>Imagenes/comedores/comedores12.png</v>
+      </c>
+      <c r="L32" t="str">
+        <f>+$H$21&amp;I32</f>
+        <v>comedores12</v>
+      </c>
+      <c r="M32" t="str">
+        <f t="shared" si="2"/>
+        <v>('comedores12','Comedor 6 puestos Europeo','N/A','$ 3.150.000','Imagenes/comedores/comedores12.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</v>
+      </c>
+      <c r="N32" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B33" t="s">
+        <v>302</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I33">
+        <v>13</v>
+      </c>
+      <c r="K33" t="str">
+        <f>$H$19&amp;$H$21&amp;I33&amp;$J$21</f>
+        <v>Imagenes/comedores/comedores13.png</v>
+      </c>
+      <c r="L33" t="str">
+        <f>+$H$21&amp;I33</f>
+        <v>comedores13</v>
+      </c>
+      <c r="M33" t="str">
+        <f t="shared" si="2"/>
+        <v>('comedores13','Comedor 8 puestos Industrial','N/A','$ 4.990.000','Imagenes/comedores/comedores13.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</v>
+      </c>
+      <c r="N33" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B34" t="s">
+        <v>303</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I34">
+        <v>14</v>
+      </c>
+      <c r="K34" t="str">
+        <f>$H$19&amp;$H$21&amp;I34&amp;$J$21</f>
+        <v>Imagenes/comedores/comedores14.png</v>
+      </c>
+      <c r="L34" t="str">
+        <f>+$H$21&amp;I34</f>
+        <v>comedores14</v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="2"/>
+        <v>('comedores14','Comedor 6 puestos Minimalista','N/A','$ 2.750.000','Imagenes/comedores/comedores14.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</v>
+      </c>
+      <c r="N34" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>281</v>
+      </c>
+      <c r="B35" t="s">
+        <v>304</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I35">
+        <v>15</v>
+      </c>
+      <c r="K35" t="str">
+        <f>$H$19&amp;$H$21&amp;I35&amp;$J$21</f>
+        <v>Imagenes/comedores/comedores15.png</v>
+      </c>
+      <c r="L35" t="str">
+        <f>+$H$21&amp;I35</f>
+        <v>comedores15</v>
+      </c>
+      <c r="M35" t="str">
+        <f t="shared" si="2"/>
+        <v>('comedores15','Comedor 6 puestos Valenciano plus','N/A','$ 4.250.000','Imagenes/comedores/comedores15.png',' Natural , Wengue ,  Caoba',' Madera , Vidrio , Metal '),</v>
+      </c>
+      <c r="N35" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="K37" t="str">
+        <f>+$H$21&amp;I21</f>
+        <v>comedores1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>252</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="K38" t="str">
+        <f t="shared" ref="K38:K51" si="3">+$H$21&amp;I22</f>
+        <v>comedores2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>253</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="K39" t="str">
+        <f t="shared" si="3"/>
+        <v>comedores3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>254</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="K40" t="str">
+        <f t="shared" si="3"/>
+        <v>comedores4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>255</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="K41" t="str">
+        <f t="shared" si="3"/>
+        <v>comedores5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>256</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H42" t="s">
+        <v>193</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" si="3"/>
+        <v>comedores6</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="K43" t="str">
+        <f t="shared" si="3"/>
+        <v>comedores7</v>
+      </c>
+      <c r="L43" t="str">
+        <f>+F42&amp;G42&amp;H42&amp;I42&amp;J42&amp;K42&amp;L42</f>
+        <v>BeigeAzulWengueGrisCaobacomedores6Plata</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="K44" t="str">
+        <f t="shared" si="3"/>
+        <v>comedores8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D45" s="1"/>
+      <c r="K45" t="str">
+        <f t="shared" si="3"/>
+        <v>comedores9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <f>+LEN(D46)</f>
+        <v>0</v>
+      </c>
+      <c r="F46" t="e">
+        <f>+RIGHT(D46,(E46-3))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K46" t="str">
+        <f t="shared" si="3"/>
+        <v>comedores10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>156</v>
+      </c>
+      <c r="E47">
+        <f t="shared" ref="E47:E75" si="4">+LEN(D47)</f>
+        <v>0</v>
+      </c>
+      <c r="F47" t="e">
+        <f t="shared" ref="F47:F75" si="5">+RIGHT(D47,(E47-3))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K47" t="str">
+        <f t="shared" si="3"/>
+        <v>comedores11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>157</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F48" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K48" t="str">
+        <f t="shared" si="3"/>
+        <v>comedores12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F49" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K49" t="str">
+        <f t="shared" si="3"/>
+        <v>comedores13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>160</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F50" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K50" t="str">
+        <f t="shared" si="3"/>
+        <v>comedores14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F51" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K51" t="str">
+        <f t="shared" si="3"/>
+        <v>comedores15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F52" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F53" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>154</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F54" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>159</v>
+      </c>
+      <c r="D55" t="s">
+        <v>124</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="F55" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> Sofá Capri</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>125</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="F56" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> Sillón Victoria</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>158</v>
+      </c>
+      <c r="D57" t="s">
+        <v>126</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="F57" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> Sofá Valencia</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>127</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="F58" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> Sillón Dublín</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>128</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="F59" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> Sofá Chicago</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>129</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> Sillón Berlín</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>130</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="F61" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> Sofá Venecia</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>131</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="F62" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> Sillón Savoy</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>132</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="F63" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> Sofá París</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>133</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="F64" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> Sillón Duke</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>155</v>
+      </c>
+      <c r="D65" t="s">
+        <v>134</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="F65" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> Sofá Florencia</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>135</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="F66" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> Sillón Oxford</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>151</v>
+      </c>
+      <c r="D67" t="s">
+        <v>136</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="F67" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> Sofá Barcelona</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>146</v>
+      </c>
+      <c r="D68" t="s">
+        <v>137</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="F68" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> Sillón Marsella</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>153</v>
+      </c>
+      <c r="D69" t="s">
+        <v>138</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="F69" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> Sofá Londres</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>147</v>
+      </c>
+      <c r="D70" t="s">
+        <v>139</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="F70" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> Sillón Zurich</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>149</v>
+      </c>
+      <c r="D71" t="s">
+        <v>140</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="F71" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> Sofá Sevilla</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>152</v>
+      </c>
+      <c r="D72" t="s">
+        <v>141</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="F72" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> Sillón Toulouse</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>142</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="F73" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> Sofá Bruselas</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>145</v>
+      </c>
+      <c r="D74" t="s">
+        <v>143</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="F74" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> Sillón Mónaco</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>150</v>
+      </c>
+      <c r="D75" t="s">
+        <v>144</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="F75" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> Sofá Ámsterdam</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D76" s="1"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D77" s="1"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D78" s="1"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D79" s="1"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="6"/>
+      <c r="B100" s="7"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="7"/>
+      <c r="E100" s="7"/>
+      <c r="F100" s="7"/>
+      <c r="G100" s="7"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="1"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="F104" s="2"/>
+      <c r="G104" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Carga version final alternativa 25-06-2023
</commit_message>
<xml_diff>
--- a/Query Base de datos.xlsx
+++ b/Query Base de datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\unificacion_proyecto_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A499E8DD-41D5-4743-8BD5-CBA84F6F1A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71250615-23C5-417B-A064-97ED94C3EA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{2A26BEC3-3C8D-473A-BF84-89C24DF24433}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2A26BEC3-3C8D-473A-BF84-89C24DF24433}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1990,7 +1990,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2037,7 +2037,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -2047,7 +2047,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2368,7 +2367,7 @@
       <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
@@ -2382,27 +2381,27 @@
     <col min="10" max="10" width="194.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="H5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
@@ -2425,7 +2424,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -2458,7 +2457,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -2491,7 +2490,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -2524,7 +2523,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -2557,23 +2556,23 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>45</v>
       </c>
       <c r="B19" s="5"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="B20" t="s">
         <v>53</v>
       </c>
@@ -2588,7 +2587,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="C21" t="s">
         <v>47</v>
       </c>
@@ -2600,7 +2599,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="C22" t="s">
         <v>48</v>
       </c>
@@ -2612,7 +2611,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="C23" t="s">
         <v>49</v>
       </c>
@@ -2624,12 +2623,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -2637,7 +2636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -2645,7 +2644,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -2653,7 +2652,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -2661,72 +2660,72 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -2741,7 +2740,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9">
       <c r="B49" t="s">
         <v>75</v>
       </c>
@@ -2753,7 +2752,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9">
       <c r="B50" t="s">
         <v>76</v>
       </c>
@@ -2765,7 +2764,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9">
       <c r="B51" t="s">
         <v>77</v>
       </c>
@@ -2777,17 +2776,17 @@
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9">
       <c r="A58" t="s">
         <v>0</v>
       </c>
@@ -2810,7 +2809,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9">
       <c r="A59" t="s">
         <v>97</v>
       </c>
@@ -2837,7 +2836,7 @@
         <v>('PRU_009','Pru alta carpinteria 2','Descripcion prueba alta carpineteria',1000000.00,'Imagenes/seccionAlcobas2 - copia.png','Azul,Blanco,Negro','Material3,Material4,Material5')</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9">
       <c r="A60" t="s">
         <v>82</v>
       </c>
@@ -2864,7 +2863,7 @@
         <v>('PRU_006','Pru Alcobas 2','Descripcion prueba alta carpinteria',1500000.00,'Imagenes/seccion alta carpinteria - copia.png','Azul,Blanco','Material1,Material2,Material4,Material5')</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9">
       <c r="A61" t="s">
         <v>83</v>
       </c>
@@ -2891,7 +2890,7 @@
         <v>('PRU_007','Pru Comedor 2','Descripcion prueba comedor',2100000.00,'Imagenes/seccionComedor - copia.png','Rojo,Blanco,Negro','Material1,Material3,Material4')</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9">
       <c r="A62" t="s">
         <v>84</v>
       </c>
@@ -2918,7 +2917,7 @@
         <v>('PRU_008','Pru Salas 2','Descripcion prueba salas',1800000.00,'Imagenes/SeccionSalas - copia.png','Rojo,Azul,Blanco,Negro','Material2,Material3,Material5')</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7">
       <c r="A83" s="6" t="s">
         <v>0</v>
       </c>
@@ -2941,7 +2940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7">
       <c r="A84" s="1" t="s">
         <v>7</v>
       </c>
@@ -2964,7 +2963,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7">
       <c r="A85" s="1" t="s">
         <v>8</v>
       </c>
@@ -2987,7 +2986,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7">
       <c r="A86" s="1" t="s">
         <v>9</v>
       </c>
@@ -3010,7 +3009,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7">
       <c r="A87" s="1" t="s">
         <v>10</v>
       </c>
@@ -3043,58 +3042,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAA30AA2-9880-4D41-820C-F91482830A46}">
   <dimension ref="A1:N104"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21:N35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="67.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>209</v>
       </c>
@@ -3102,17 +3101,17 @@
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="F10" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>580</v>
       </c>
@@ -3120,7 +3119,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -3129,7 +3128,7 @@
         <v>('VALUES','','','','','',''),</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="H19" t="s">
         <v>175</v>
       </c>
@@ -3137,7 +3136,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="A20" s="6" t="s">
         <v>100</v>
       </c>
@@ -3166,7 +3165,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
         <v>109</v>
       </c>
@@ -3213,7 +3212,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
         <v>110</v>
       </c>
@@ -3247,14 +3246,14 @@
         <v>salas2</v>
       </c>
       <c r="M22" t="str">
-        <f t="shared" ref="M22:N35" si="3">+"('"&amp;A22&amp;"'"&amp;$L$20&amp;"'"&amp;B22&amp;"'"&amp;$L$20&amp;"'"&amp;C22&amp;"'"&amp;$L$20&amp;"'"&amp;D22&amp;"'"&amp;$L$20&amp;"'"&amp;E22&amp;"'),"</f>
+        <f t="shared" ref="M22:M35" si="3">+"('"&amp;A22&amp;"'"&amp;$L$20&amp;"'"&amp;B22&amp;"'"&amp;$L$20&amp;"'"&amp;C22&amp;"'"&amp;$L$20&amp;"'"&amp;D22&amp;"'"&amp;$L$20&amp;"'"&amp;E22&amp;"'),"</f>
         <v>('salas2','Sillón Berlín','N/A','$ 1.800.000','Imagenes/salas/salas2.png'),</v>
       </c>
       <c r="N22" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
         <v>111</v>
       </c>
@@ -3295,7 +3294,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
         <v>112</v>
       </c>
@@ -3336,7 +3335,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
         <v>113</v>
       </c>
@@ -3377,7 +3376,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
         <v>114</v>
       </c>
@@ -3418,7 +3417,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
         <v>115</v>
       </c>
@@ -3459,7 +3458,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
         <v>116</v>
       </c>
@@ -3500,7 +3499,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14">
       <c r="A29" s="8" t="s">
         <v>117</v>
       </c>
@@ -3541,7 +3540,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
         <v>118</v>
       </c>
@@ -3582,7 +3581,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
         <v>119</v>
       </c>
@@ -3623,7 +3622,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
         <v>120</v>
       </c>
@@ -3664,7 +3663,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14">
       <c r="A33" s="1" t="s">
         <v>121</v>
       </c>
@@ -3705,7 +3704,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14">
       <c r="A34" s="1" t="s">
         <v>122</v>
       </c>
@@ -3746,7 +3745,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
         <v>123</v>
       </c>
@@ -3787,7 +3786,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -3796,7 +3795,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -3805,7 +3804,7 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
         <v>236</v>
       </c>
@@ -3816,7 +3815,7 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
         <v>237</v>
       </c>
@@ -3827,7 +3826,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
         <v>238</v>
       </c>
@@ -3838,7 +3837,7 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
         <v>239</v>
       </c>
@@ -3849,7 +3848,7 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
         <v>240</v>
       </c>
@@ -3879,7 +3878,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14">
       <c r="A43" t="s">
         <v>62</v>
       </c>
@@ -3894,7 +3893,7 @@
         <v>BeigeAzulWengueGrisCaobaBlancoPlata</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -3902,10 +3901,10 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14">
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14">
       <c r="E46">
         <f>+LEN(D46)</f>
         <v>0</v>
@@ -3915,7 +3914,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14">
       <c r="A47" t="s">
         <v>156</v>
       </c>
@@ -3928,7 +3927,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14">
       <c r="A48" t="s">
         <v>157</v>
       </c>
@@ -3941,7 +3940,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="E49">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3951,7 +3950,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>160</v>
       </c>
@@ -3964,7 +3963,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="E51">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3974,7 +3973,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="E52">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3984,7 +3983,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="E53">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3994,7 +3993,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>154</v>
       </c>
@@ -4007,7 +4006,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>159</v>
       </c>
@@ -4023,7 +4022,7 @@
         <v xml:space="preserve"> Sofá Capri</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="D56" t="s">
         <v>125</v>
       </c>
@@ -4036,7 +4035,7 @@
         <v xml:space="preserve"> Sillón Victoria</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>158</v>
       </c>
@@ -4052,7 +4051,7 @@
         <v xml:space="preserve"> Sofá Valencia</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="D58" t="s">
         <v>127</v>
       </c>
@@ -4065,7 +4064,7 @@
         <v xml:space="preserve"> Sillón Dublín</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="D59" t="s">
         <v>128</v>
       </c>
@@ -4078,7 +4077,7 @@
         <v xml:space="preserve"> Sofá Chicago</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="D60" t="s">
         <v>129</v>
       </c>
@@ -4091,7 +4090,7 @@
         <v xml:space="preserve"> Sillón Berlín</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="D61" t="s">
         <v>130</v>
       </c>
@@ -4104,7 +4103,7 @@
         <v xml:space="preserve"> Sofá Venecia</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="D62" t="s">
         <v>131</v>
       </c>
@@ -4117,7 +4116,7 @@
         <v xml:space="preserve"> Sillón Savoy</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="D63" t="s">
         <v>132</v>
       </c>
@@ -4130,7 +4129,7 @@
         <v xml:space="preserve"> Sofá París</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="D64" t="s">
         <v>133</v>
       </c>
@@ -4143,7 +4142,7 @@
         <v xml:space="preserve"> Sillón Duke</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
         <v>155</v>
       </c>
@@ -4159,7 +4158,7 @@
         <v xml:space="preserve"> Sofá Florencia</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6">
       <c r="D66" t="s">
         <v>135</v>
       </c>
@@ -4172,7 +4171,7 @@
         <v xml:space="preserve"> Sillón Oxford</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
         <v>151</v>
       </c>
@@ -4188,7 +4187,7 @@
         <v xml:space="preserve"> Sofá Barcelona</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
         <v>146</v>
       </c>
@@ -4204,7 +4203,7 @@
         <v xml:space="preserve"> Sillón Marsella</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
         <v>153</v>
       </c>
@@ -4220,7 +4219,7 @@
         <v xml:space="preserve"> Sofá Londres</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
         <v>147</v>
       </c>
@@ -4236,7 +4235,7 @@
         <v xml:space="preserve"> Sillón Zurich</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
         <v>149</v>
       </c>
@@ -4252,7 +4251,7 @@
         <v xml:space="preserve"> Sofá Sevilla</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
         <v>152</v>
       </c>
@@ -4268,7 +4267,7 @@
         <v xml:space="preserve"> Sillón Toulouse</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6">
       <c r="D73" t="s">
         <v>142</v>
       </c>
@@ -4281,7 +4280,7 @@
         <v xml:space="preserve"> Sofá Bruselas</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
         <v>145</v>
       </c>
@@ -4297,7 +4296,7 @@
         <v xml:space="preserve"> Sillón Mónaco</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
         <v>150</v>
       </c>
@@ -4313,19 +4312,19 @@
         <v xml:space="preserve"> Sofá Ámsterdam</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6">
       <c r="D76" s="1"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6">
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6">
       <c r="D78" s="1"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6">
       <c r="D79" s="1"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7">
       <c r="A100" s="6"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -4334,7 +4333,7 @@
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7">
       <c r="A101" s="1"/>
       <c r="B101" s="2"/>
       <c r="C101" s="1"/>
@@ -4342,7 +4341,7 @@
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -4350,7 +4349,7 @@
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -4358,7 +4357,7 @@
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -4383,7 +4382,7 @@
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="31.42578125" customWidth="1"/>
     <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
@@ -4392,47 +4391,47 @@
     <col min="13" max="13" width="100.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>209</v>
       </c>
@@ -4440,17 +4439,17 @@
         <v>245</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="E10" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>581</v>
       </c>
@@ -4458,12 +4457,12 @@
         <v>304</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="H19" t="s">
         <v>244</v>
       </c>
@@ -4471,7 +4470,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="A20" s="6" t="s">
         <v>100</v>
       </c>
@@ -4500,7 +4499,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
         <v>251</v>
       </c>
@@ -4547,7 +4546,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
         <v>252</v>
       </c>
@@ -4581,14 +4580,14 @@
         <v>comedores2</v>
       </c>
       <c r="M22" t="str">
-        <f t="shared" ref="M22:N35" si="2">+"('"&amp;A22&amp;"'"&amp;$L$20&amp;"'"&amp;B22&amp;"'"&amp;$L$20&amp;"'"&amp;C22&amp;"'"&amp;$L$20&amp;"'"&amp;D22&amp;"'"&amp;$L$20&amp;"'"&amp;E22&amp;"'),"</f>
+        <f t="shared" ref="M22:M35" si="2">+"('"&amp;A22&amp;"'"&amp;$L$20&amp;"'"&amp;B22&amp;"'"&amp;$L$20&amp;"'"&amp;C22&amp;"'"&amp;$L$20&amp;"'"&amp;D22&amp;"'"&amp;$L$20&amp;"'"&amp;E22&amp;"'),"</f>
         <v>('comedores2','Comedor 6 puestos Sevilla','N/A','$ 2.830.000','Imagenes/comedores/comedores2.png'),</v>
       </c>
       <c r="N22" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
         <v>253</v>
       </c>
@@ -4629,7 +4628,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
         <v>254</v>
       </c>
@@ -4670,7 +4669,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
         <v>255</v>
       </c>
@@ -4711,7 +4710,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
         <v>256</v>
       </c>
@@ -4752,7 +4751,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
         <v>257</v>
       </c>
@@ -4793,7 +4792,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
         <v>258</v>
       </c>
@@ -4834,7 +4833,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14">
       <c r="A29" s="8" t="s">
         <v>259</v>
       </c>
@@ -4875,7 +4874,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
         <v>260</v>
       </c>
@@ -4916,7 +4915,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
         <v>261</v>
       </c>
@@ -4957,7 +4956,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
         <v>262</v>
       </c>
@@ -4998,7 +4997,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14">
       <c r="A33" s="1" t="s">
         <v>263</v>
       </c>
@@ -5039,7 +5038,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14">
       <c r="A34" s="1" t="s">
         <v>264</v>
       </c>
@@ -5080,7 +5079,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
         <v>265</v>
       </c>
@@ -5121,7 +5120,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -5130,7 +5129,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -5143,7 +5142,7 @@
         <v>comedores1</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
         <v>236</v>
       </c>
@@ -5158,7 +5157,7 @@
         <v>comedores2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
         <v>237</v>
       </c>
@@ -5173,7 +5172,7 @@
         <v>comedores3</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
         <v>238</v>
       </c>
@@ -5188,7 +5187,7 @@
         <v>comedores4</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
         <v>239</v>
       </c>
@@ -5203,7 +5202,7 @@
         <v>comedores5</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
         <v>240</v>
       </c>
@@ -5234,7 +5233,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14">
       <c r="A43" t="s">
         <v>62</v>
       </c>
@@ -5253,7 +5252,7 @@
         <v>BeigeAzulWengueGrisCaobacomedores6Plata</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -5265,14 +5264,14 @@
         <v>comedores8</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14">
       <c r="D45" s="1"/>
       <c r="K45" t="str">
         <f t="shared" si="3"/>
         <v>comedores9</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14">
       <c r="E46">
         <f>+LEN(D46)</f>
         <v>0</v>
@@ -5286,7 +5285,7 @@
         <v>comedores10</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14">
       <c r="A47" t="s">
         <v>156</v>
       </c>
@@ -5303,7 +5302,7 @@
         <v>comedores11</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14">
       <c r="A48" t="s">
         <v>157</v>
       </c>
@@ -5320,7 +5319,7 @@
         <v>comedores12</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11">
       <c r="E49">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5334,7 +5333,7 @@
         <v>comedores13</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11">
       <c r="A50" t="s">
         <v>160</v>
       </c>
@@ -5351,7 +5350,7 @@
         <v>comedores14</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11">
       <c r="E51">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5365,7 +5364,7 @@
         <v>comedores15</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11">
       <c r="E52">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5375,7 +5374,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11">
       <c r="E53">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5385,7 +5384,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11">
       <c r="A54" t="s">
         <v>154</v>
       </c>
@@ -5398,7 +5397,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11">
       <c r="A55" t="s">
         <v>159</v>
       </c>
@@ -5414,7 +5413,7 @@
         <v xml:space="preserve"> Sofá Capri</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11">
       <c r="D56" t="s">
         <v>125</v>
       </c>
@@ -5427,7 +5426,7 @@
         <v xml:space="preserve"> Sillón Victoria</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11">
       <c r="A57" t="s">
         <v>158</v>
       </c>
@@ -5443,7 +5442,7 @@
         <v xml:space="preserve"> Sofá Valencia</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11">
       <c r="D58" t="s">
         <v>127</v>
       </c>
@@ -5456,7 +5455,7 @@
         <v xml:space="preserve"> Sillón Dublín</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11">
       <c r="D59" t="s">
         <v>128</v>
       </c>
@@ -5469,7 +5468,7 @@
         <v xml:space="preserve"> Sofá Chicago</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11">
       <c r="D60" t="s">
         <v>129</v>
       </c>
@@ -5482,7 +5481,7 @@
         <v xml:space="preserve"> Sillón Berlín</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11">
       <c r="D61" t="s">
         <v>130</v>
       </c>
@@ -5495,7 +5494,7 @@
         <v xml:space="preserve"> Sofá Venecia</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11">
       <c r="D62" t="s">
         <v>131</v>
       </c>
@@ -5508,7 +5507,7 @@
         <v xml:space="preserve"> Sillón Savoy</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11">
       <c r="D63" t="s">
         <v>132</v>
       </c>
@@ -5521,7 +5520,7 @@
         <v xml:space="preserve"> Sofá París</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11">
       <c r="D64" t="s">
         <v>133</v>
       </c>
@@ -5534,7 +5533,7 @@
         <v xml:space="preserve"> Sillón Duke</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
         <v>155</v>
       </c>
@@ -5550,7 +5549,7 @@
         <v xml:space="preserve"> Sofá Florencia</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6">
       <c r="D66" t="s">
         <v>135</v>
       </c>
@@ -5563,7 +5562,7 @@
         <v xml:space="preserve"> Sillón Oxford</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
         <v>151</v>
       </c>
@@ -5579,7 +5578,7 @@
         <v xml:space="preserve"> Sofá Barcelona</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
         <v>146</v>
       </c>
@@ -5595,7 +5594,7 @@
         <v xml:space="preserve"> Sillón Marsella</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
         <v>153</v>
       </c>
@@ -5611,7 +5610,7 @@
         <v xml:space="preserve"> Sofá Londres</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
         <v>147</v>
       </c>
@@ -5627,7 +5626,7 @@
         <v xml:space="preserve"> Sillón Zurich</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
         <v>149</v>
       </c>
@@ -5643,7 +5642,7 @@
         <v xml:space="preserve"> Sofá Sevilla</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
         <v>152</v>
       </c>
@@ -5659,7 +5658,7 @@
         <v xml:space="preserve"> Sillón Toulouse</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6">
       <c r="D73" t="s">
         <v>142</v>
       </c>
@@ -5672,7 +5671,7 @@
         <v xml:space="preserve"> Sofá Bruselas</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
         <v>145</v>
       </c>
@@ -5688,7 +5687,7 @@
         <v xml:space="preserve"> Sillón Mónaco</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
         <v>150</v>
       </c>
@@ -5704,19 +5703,19 @@
         <v xml:space="preserve"> Sofá Ámsterdam</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6">
       <c r="D76" s="1"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6">
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6">
       <c r="D78" s="1"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6">
       <c r="D79" s="1"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7">
       <c r="A100" s="6"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -5725,7 +5724,7 @@
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7">
       <c r="A101" s="1"/>
       <c r="B101" s="2"/>
       <c r="C101" s="1"/>
@@ -5733,7 +5732,7 @@
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -5741,7 +5740,7 @@
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -5749,7 +5748,7 @@
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -5771,7 +5770,7 @@
       <selection activeCell="N21" sqref="N21:N35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="31.42578125" customWidth="1"/>
     <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
@@ -5784,47 +5783,47 @@
     <col min="13" max="13" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>209</v>
       </c>
@@ -5832,27 +5831,27 @@
         <v>368</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="E10" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="H19" t="s">
         <v>322</v>
       </c>
@@ -5860,7 +5859,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="A20" s="6" t="s">
         <v>100</v>
       </c>
@@ -5889,7 +5888,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
         <v>307</v>
       </c>
@@ -5936,7 +5935,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
         <v>308</v>
       </c>
@@ -5970,14 +5969,14 @@
         <v>alcobas2</v>
       </c>
       <c r="M22" t="str">
-        <f t="shared" ref="M22:N35" si="2">+"('"&amp;A22&amp;"'"&amp;$L$20&amp;"'"&amp;B22&amp;"'"&amp;$L$20&amp;"'"&amp;C22&amp;"'"&amp;$L$20&amp;"'"&amp;D22&amp;"'"&amp;$L$20&amp;"'"&amp;E22&amp;"'),"</f>
+        <f t="shared" ref="M22:M35" si="2">+"('"&amp;A22&amp;"'"&amp;$L$20&amp;"'"&amp;B22&amp;"'"&amp;$L$20&amp;"'"&amp;C22&amp;"'"&amp;$L$20&amp;"'"&amp;D22&amp;"'"&amp;$L$20&amp;"'"&amp;E22&amp;"'),"</f>
         <v>('alcobas2','Juego alcoba Brooklyn','N/A','$ 2.990.000','Imagenes/alcobas/alcobas2.png'),</v>
       </c>
       <c r="N22" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
         <v>309</v>
       </c>
@@ -6018,7 +6017,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
         <v>310</v>
       </c>
@@ -6059,7 +6058,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
         <v>311</v>
       </c>
@@ -6100,7 +6099,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
         <v>312</v>
       </c>
@@ -6141,7 +6140,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
         <v>313</v>
       </c>
@@ -6182,7 +6181,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
         <v>314</v>
       </c>
@@ -6223,7 +6222,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14">
       <c r="A29" s="8" t="s">
         <v>315</v>
       </c>
@@ -6264,7 +6263,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
         <v>316</v>
       </c>
@@ -6305,7 +6304,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
         <v>317</v>
       </c>
@@ -6346,7 +6345,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
         <v>318</v>
       </c>
@@ -6387,7 +6386,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14">
       <c r="A33" s="1" t="s">
         <v>319</v>
       </c>
@@ -6428,7 +6427,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14">
       <c r="A34" s="1" t="s">
         <v>320</v>
       </c>
@@ -6469,7 +6468,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
         <v>321</v>
       </c>
@@ -6510,7 +6509,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -6519,7 +6518,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -6532,7 +6531,7 @@
         <v>alcobas1</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
         <v>236</v>
       </c>
@@ -6547,7 +6546,7 @@
         <v>alcobas2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
         <v>237</v>
       </c>
@@ -6562,7 +6561,7 @@
         <v>alcobas3</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
         <v>238</v>
       </c>
@@ -6577,7 +6576,7 @@
         <v>alcobas4</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
         <v>239</v>
       </c>
@@ -6592,7 +6591,7 @@
         <v>alcobas5</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
         <v>240</v>
       </c>
@@ -6623,7 +6622,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14">
       <c r="A43" t="s">
         <v>62</v>
       </c>
@@ -6642,7 +6641,7 @@
         <v>BeigeAzulWengueGrisCaobaalcobas6Plata</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -6654,62 +6653,62 @@
         <v>alcobas8</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14">
       <c r="D45" s="1"/>
       <c r="K45" t="str">
         <f t="shared" si="3"/>
         <v>alcobas9</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14">
       <c r="K46" t="str">
         <f t="shared" si="3"/>
         <v>alcobas10</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14">
       <c r="K47" t="str">
         <f t="shared" si="3"/>
         <v>alcobas11</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14">
       <c r="K48" t="str">
         <f t="shared" si="3"/>
         <v>alcobas12</v>
       </c>
     </row>
-    <row r="49" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="11:11">
       <c r="K49" t="str">
         <f t="shared" si="3"/>
         <v>alcobas13</v>
       </c>
     </row>
-    <row r="50" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="11:11">
       <c r="K50" t="str">
         <f t="shared" si="3"/>
         <v>alcobas14</v>
       </c>
     </row>
-    <row r="51" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="11:11">
       <c r="K51" t="str">
         <f t="shared" si="3"/>
         <v>alcobas15</v>
       </c>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:4">
       <c r="D76" s="1"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:4">
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:4">
       <c r="D78" s="1"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:4">
       <c r="D79" s="1"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7">
       <c r="A100" s="6"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -6718,7 +6717,7 @@
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7">
       <c r="A101" s="1"/>
       <c r="B101" s="2"/>
       <c r="C101" s="1"/>
@@ -6726,7 +6725,7 @@
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -6734,7 +6733,7 @@
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -6742,7 +6741,7 @@
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -6764,7 +6763,7 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="31.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
@@ -6779,47 +6778,47 @@
     <col min="13" max="13" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>209</v>
       </c>
@@ -6827,17 +6826,17 @@
         <v>372</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="F10" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>583</v>
       </c>
@@ -6845,12 +6844,12 @@
         <v>429</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="H19" t="s">
         <v>373</v>
       </c>
@@ -6858,7 +6857,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="A20" s="6" t="s">
         <v>100</v>
       </c>
@@ -6887,7 +6886,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
         <v>375</v>
       </c>
@@ -6934,7 +6933,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
         <v>376</v>
       </c>
@@ -6968,14 +6967,14 @@
         <v>cocina2</v>
       </c>
       <c r="M22" t="str">
-        <f t="shared" ref="M22:N35" si="2">+"('"&amp;A22&amp;"'"&amp;$L$20&amp;"'"&amp;B22&amp;"'"&amp;$L$20&amp;"'"&amp;C22&amp;"'"&amp;$L$20&amp;"'"&amp;D22&amp;"'"&amp;$L$20&amp;"'"&amp;E22&amp;"'),"</f>
+        <f t="shared" ref="M22:M35" si="2">+"('"&amp;A22&amp;"'"&amp;$L$20&amp;"'"&amp;B22&amp;"'"&amp;$L$20&amp;"'"&amp;C22&amp;"'"&amp;$L$20&amp;"'"&amp;D22&amp;"'"&amp;$L$20&amp;"'"&amp;E22&amp;"'),"</f>
         <v>('cocina2','Cocina Nevada en L','N/A','Desde $ 6.500.000','Imagenes/cocinas/cocina2.png'),</v>
       </c>
       <c r="N22" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
         <v>377</v>
       </c>
@@ -7016,7 +7015,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
         <v>378</v>
       </c>
@@ -7057,7 +7056,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
         <v>379</v>
       </c>
@@ -7098,7 +7097,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
         <v>380</v>
       </c>
@@ -7139,7 +7138,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
         <v>381</v>
       </c>
@@ -7180,7 +7179,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
         <v>382</v>
       </c>
@@ -7221,7 +7220,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14">
       <c r="A29" s="8" t="s">
         <v>383</v>
       </c>
@@ -7262,7 +7261,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
         <v>384</v>
       </c>
@@ -7303,7 +7302,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
         <v>385</v>
       </c>
@@ -7344,7 +7343,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
         <v>386</v>
       </c>
@@ -7385,7 +7384,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14">
       <c r="A33" s="1" t="s">
         <v>387</v>
       </c>
@@ -7426,7 +7425,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14">
       <c r="A34" s="1" t="s">
         <v>388</v>
       </c>
@@ -7467,7 +7466,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
         <v>389</v>
       </c>
@@ -7508,7 +7507,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -7517,7 +7516,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -7533,7 +7532,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
         <v>236</v>
       </c>
@@ -7548,7 +7547,7 @@
         <v>cocina2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
         <v>237</v>
       </c>
@@ -7563,7 +7562,7 @@
         <v>cocina3</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
         <v>238</v>
       </c>
@@ -7578,7 +7577,7 @@
         <v>cocina4</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
         <v>239</v>
       </c>
@@ -7593,7 +7592,7 @@
         <v>cocina5</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
         <v>240</v>
       </c>
@@ -7624,7 +7623,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14">
       <c r="A43" t="s">
         <v>62</v>
       </c>
@@ -7643,7 +7642,7 @@
         <v>BeigeAzulWengueGrisCaobacocina6Plata</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -7655,62 +7654,62 @@
         <v>cocina8</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14">
       <c r="D45" s="1"/>
       <c r="K45" t="str">
         <f t="shared" si="3"/>
         <v>cocina9</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14">
       <c r="K46" t="str">
         <f t="shared" si="3"/>
         <v>cocina10</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14">
       <c r="K47" t="str">
         <f t="shared" si="3"/>
         <v>cocina11</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14">
       <c r="K48" t="str">
         <f t="shared" si="3"/>
         <v>cocina12</v>
       </c>
     </row>
-    <row r="49" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="11:11">
       <c r="K49" t="str">
         <f t="shared" si="3"/>
         <v>cocina13</v>
       </c>
     </row>
-    <row r="50" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="11:11">
       <c r="K50" t="str">
         <f t="shared" si="3"/>
         <v>cocina14</v>
       </c>
     </row>
-    <row r="51" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="11:11">
       <c r="K51" t="str">
         <f t="shared" si="3"/>
         <v>cocina15</v>
       </c>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:4">
       <c r="D76" s="1"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:4">
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:4">
       <c r="D78" s="1"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:4">
       <c r="D79" s="1"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7">
       <c r="A100" s="6"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -7719,7 +7718,7 @@
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7">
       <c r="A101" s="1"/>
       <c r="B101" s="2"/>
       <c r="C101" s="1"/>
@@ -7727,7 +7726,7 @@
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -7735,7 +7734,7 @@
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -7743,7 +7742,7 @@
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -7765,7 +7764,7 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="43.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
@@ -7779,47 +7778,47 @@
     <col min="13" max="13" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>209</v>
       </c>
@@ -7827,27 +7826,27 @@
         <v>372</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="E10" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="H19" t="s">
         <v>431</v>
       </c>
@@ -7855,7 +7854,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="A20" s="6" t="s">
         <v>100</v>
       </c>
@@ -7884,7 +7883,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
         <v>433</v>
       </c>
@@ -7931,7 +7930,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
         <v>434</v>
       </c>
@@ -7965,14 +7964,14 @@
         <v>estudio2</v>
       </c>
       <c r="M22" t="str">
-        <f t="shared" ref="M22:N35" si="2">+"('"&amp;A22&amp;"'"&amp;$L$20&amp;"'"&amp;B22&amp;"'"&amp;$L$20&amp;"'"&amp;C22&amp;"'"&amp;$L$20&amp;"'"&amp;D22&amp;"'"&amp;$L$20&amp;"'"&amp;E22&amp;"'),"</f>
+        <f t="shared" ref="M22:M35" si="2">+"('"&amp;A22&amp;"'"&amp;$L$20&amp;"'"&amp;B22&amp;"'"&amp;$L$20&amp;"'"&amp;C22&amp;"'"&amp;$L$20&amp;"'"&amp;D22&amp;"'"&amp;$L$20&amp;"'"&amp;E22&amp;"'),"</f>
         <v>('estudio2','Escritorio empotrado y mueble superior Alaska','N/A','Desde $ 3.500.000','Imagenes/cuartos_de_estudio/estudio2.png'),</v>
       </c>
       <c r="N22" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
         <v>435</v>
       </c>
@@ -8013,7 +8012,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
         <v>436</v>
       </c>
@@ -8054,7 +8053,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
         <v>437</v>
       </c>
@@ -8095,7 +8094,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
         <v>438</v>
       </c>
@@ -8136,7 +8135,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
         <v>439</v>
       </c>
@@ -8177,7 +8176,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
         <v>440</v>
       </c>
@@ -8218,7 +8217,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14">
       <c r="A29" s="8" t="s">
         <v>441</v>
       </c>
@@ -8259,7 +8258,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
         <v>442</v>
       </c>
@@ -8300,7 +8299,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
         <v>443</v>
       </c>
@@ -8341,7 +8340,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
         <v>444</v>
       </c>
@@ -8382,7 +8381,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14">
       <c r="A33" s="1" t="s">
         <v>445</v>
       </c>
@@ -8423,7 +8422,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14">
       <c r="A34" s="1" t="s">
         <v>446</v>
       </c>
@@ -8464,7 +8463,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
         <v>447</v>
       </c>
@@ -8505,7 +8504,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -8514,7 +8513,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -8530,7 +8529,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
         <v>236</v>
       </c>
@@ -8545,7 +8544,7 @@
         <v>estudio2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
         <v>237</v>
       </c>
@@ -8560,7 +8559,7 @@
         <v>estudio3</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
         <v>238</v>
       </c>
@@ -8575,7 +8574,7 @@
         <v>estudio4</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
         <v>239</v>
       </c>
@@ -8590,7 +8589,7 @@
         <v>estudio5</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
         <v>240</v>
       </c>
@@ -8621,7 +8620,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14">
       <c r="A43" t="s">
         <v>62</v>
       </c>
@@ -8640,7 +8639,7 @@
         <v>BeigeAzulWengueGrisCaobaestudio6Plata</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -8652,62 +8651,62 @@
         <v>estudio8</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14">
       <c r="D45" s="1"/>
       <c r="K45" t="str">
         <f t="shared" si="3"/>
         <v>estudio9</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14">
       <c r="K46" t="str">
         <f t="shared" si="3"/>
         <v>estudio10</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14">
       <c r="K47" t="str">
         <f t="shared" si="3"/>
         <v>estudio11</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14">
       <c r="K48" t="str">
         <f t="shared" si="3"/>
         <v>estudio12</v>
       </c>
     </row>
-    <row r="49" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="11:11">
       <c r="K49" t="str">
         <f t="shared" si="3"/>
         <v>estudio13</v>
       </c>
     </row>
-    <row r="50" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="11:11">
       <c r="K50" t="str">
         <f t="shared" si="3"/>
         <v>estudio14</v>
       </c>
     </row>
-    <row r="51" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="11:11">
       <c r="K51" t="str">
         <f t="shared" si="3"/>
         <v>estudio15</v>
       </c>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:4">
       <c r="D76" s="1"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:4">
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:4">
       <c r="D78" s="1"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:4">
       <c r="D79" s="1"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7">
       <c r="A100" s="6"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -8716,7 +8715,7 @@
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7">
       <c r="A101" s="1"/>
       <c r="B101" s="2"/>
       <c r="C101" s="1"/>
@@ -8724,7 +8723,7 @@
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -8732,7 +8731,7 @@
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -8740,7 +8739,7 @@
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -8762,7 +8761,7 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="43.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
@@ -8776,47 +8775,47 @@
     <col min="13" max="13" width="112.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>209</v>
       </c>
@@ -8824,27 +8823,27 @@
         <v>372</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="E10" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+    <row r="18" spans="1:14">
+      <c r="A18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="H19" t="s">
         <v>510</v>
       </c>
@@ -8852,7 +8851,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="A20" s="6" t="s">
         <v>100</v>
       </c>
@@ -8881,7 +8880,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
         <v>495</v>
       </c>
@@ -8928,7 +8927,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
         <v>496</v>
       </c>
@@ -8962,14 +8961,14 @@
         <v>biblioteca2</v>
       </c>
       <c r="M22" t="str">
-        <f t="shared" ref="M22:N35" si="2">+"('"&amp;A22&amp;"'"&amp;$L$20&amp;"'"&amp;B22&amp;"'"&amp;$L$20&amp;"'"&amp;C22&amp;"'"&amp;$L$20&amp;"'"&amp;D22&amp;"'"&amp;$L$20&amp;"'"&amp;E22&amp;"'),"</f>
+        <f t="shared" ref="M22:M35" si="2">+"('"&amp;A22&amp;"'"&amp;$L$20&amp;"'"&amp;B22&amp;"'"&amp;$L$20&amp;"'"&amp;C22&amp;"'"&amp;$L$20&amp;"'"&amp;D22&amp;"'"&amp;$L$20&amp;"'"&amp;E22&amp;"'),"</f>
         <v>('biblioteca2','Biblioteca Ceniza Basic','N/A','Desde $ 3.700.000','Imagenes/bibliotecas/biblioteca2.png'),</v>
       </c>
       <c r="N22" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
         <v>497</v>
       </c>
@@ -9010,7 +9009,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
         <v>498</v>
       </c>
@@ -9051,7 +9050,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
         <v>499</v>
       </c>
@@ -9092,7 +9091,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
         <v>500</v>
       </c>
@@ -9133,7 +9132,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
         <v>501</v>
       </c>
@@ -9174,7 +9173,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
         <v>502</v>
       </c>
@@ -9215,7 +9214,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14">
       <c r="A29" s="8" t="s">
         <v>503</v>
       </c>
@@ -9256,7 +9255,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
         <v>504</v>
       </c>
@@ -9297,7 +9296,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
         <v>505</v>
       </c>
@@ -9338,7 +9337,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
         <v>506</v>
       </c>
@@ -9379,7 +9378,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14">
       <c r="A33" s="1" t="s">
         <v>507</v>
       </c>
@@ -9420,7 +9419,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14">
       <c r="A34" s="1" t="s">
         <v>508</v>
       </c>
@@ -9461,7 +9460,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
         <v>509</v>
       </c>
@@ -9502,7 +9501,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -9511,7 +9510,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -9527,7 +9526,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
         <v>236</v>
       </c>
@@ -9542,7 +9541,7 @@
         <v>biblioteca2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
         <v>237</v>
       </c>
@@ -9557,7 +9556,7 @@
         <v>biblioteca3</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
         <v>238</v>
       </c>
@@ -9572,7 +9571,7 @@
         <v>biblioteca4</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
         <v>239</v>
       </c>
@@ -9587,7 +9586,7 @@
         <v>biblioteca5</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
         <v>240</v>
       </c>
@@ -9618,7 +9617,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14">
       <c r="A43" t="s">
         <v>62</v>
       </c>
@@ -9637,7 +9636,7 @@
         <v>BeigeAzulWengueGrisCaobabiblioteca6Plata</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -9649,62 +9648,62 @@
         <v>biblioteca8</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14">
       <c r="D45" s="1"/>
       <c r="K45" t="str">
         <f t="shared" si="3"/>
         <v>biblioteca9</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14">
       <c r="K46" t="str">
         <f t="shared" si="3"/>
         <v>biblioteca10</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14">
       <c r="K47" t="str">
         <f t="shared" si="3"/>
         <v>biblioteca11</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14">
       <c r="K48" t="str">
         <f t="shared" si="3"/>
         <v>biblioteca12</v>
       </c>
     </row>
-    <row r="49" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="11:11">
       <c r="K49" t="str">
         <f t="shared" si="3"/>
         <v>biblioteca13</v>
       </c>
     </row>
-    <row r="50" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="11:11">
       <c r="K50" t="str">
         <f t="shared" si="3"/>
         <v>biblioteca14</v>
       </c>
     </row>
-    <row r="51" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="11:11">
       <c r="K51" t="str">
         <f t="shared" si="3"/>
         <v>biblioteca15</v>
       </c>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:4">
       <c r="D76" s="1"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:4">
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:4">
       <c r="D78" s="1"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:4">
       <c r="D79" s="1"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7">
       <c r="A100" s="6"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -9713,7 +9712,7 @@
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7">
       <c r="A101" s="1"/>
       <c r="B101" s="2"/>
       <c r="C101" s="1"/>
@@ -9721,7 +9720,7 @@
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -9729,7 +9728,7 @@
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -9737,7 +9736,7 @@
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -9755,11 +9754,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3698C7D6-D365-46C9-A959-8B3DAC310AB3}">
   <dimension ref="A1:N104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N21" sqref="N21:N35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="37.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
@@ -9772,47 +9771,47 @@
     <col min="13" max="13" width="108.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>209</v>
       </c>
@@ -9820,27 +9819,27 @@
         <v>372</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="E10" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="H19" t="s">
         <v>510</v>
       </c>
@@ -9848,7 +9847,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="A20" s="6" t="s">
         <v>100</v>
       </c>
@@ -9877,7 +9876,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
         <v>500</v>
       </c>
@@ -9924,7 +9923,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="A22" s="8" t="s">
         <v>441</v>
       </c>
@@ -9958,14 +9957,14 @@
         <v>biblioteca2</v>
       </c>
       <c r="M22" t="str">
-        <f t="shared" ref="M22:N35" si="2">+"('"&amp;A22&amp;"'"&amp;$L$20&amp;"'"&amp;B22&amp;"'"&amp;$L$20&amp;"'"&amp;C22&amp;"'"&amp;$L$20&amp;"'"&amp;D22&amp;"'"&amp;$L$20&amp;"'"&amp;E22&amp;"'),"</f>
+        <f t="shared" ref="M22:M35" si="2">+"('"&amp;A22&amp;"'"&amp;$L$20&amp;"'"&amp;B22&amp;"'"&amp;$L$20&amp;"'"&amp;C22&amp;"'"&amp;$L$20&amp;"'"&amp;D22&amp;"'"&amp;$L$20&amp;"'"&amp;E22&amp;"'),"</f>
         <v>('estudio9','Escritorio sencillo Vintage','N/A','Desde $ 1.500.000','Imagenes/cuartos_de_estudio/estudio9.png'),</v>
       </c>
       <c r="N22" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
         <v>380</v>
       </c>
@@ -10006,7 +10005,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14">
       <c r="A24" s="8" t="s">
         <v>503</v>
       </c>
@@ -10047,7 +10046,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
         <v>495</v>
       </c>
@@ -10088,7 +10087,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
         <v>442</v>
       </c>
@@ -10129,7 +10128,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
         <v>498</v>
       </c>
@@ -10170,7 +10169,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
         <v>505</v>
       </c>
@@ -10211,7 +10210,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14">
       <c r="A29" s="1" t="s">
         <v>384</v>
       </c>
@@ -10252,7 +10251,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
         <v>497</v>
       </c>
@@ -10293,7 +10292,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
         <v>508</v>
       </c>
@@ -10334,7 +10333,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
         <v>496</v>
       </c>
@@ -10375,7 +10374,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14">
       <c r="A33" s="1" t="s">
         <v>502</v>
       </c>
@@ -10416,7 +10415,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14">
       <c r="A34" s="1" t="s">
         <v>385</v>
       </c>
@@ -10457,7 +10456,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14">
       <c r="A35" s="1" t="s">
         <v>443</v>
       </c>
@@ -10498,7 +10497,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -10507,7 +10506,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -10523,7 +10522,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
         <v>236</v>
       </c>
@@ -10538,7 +10537,7 @@
         <v>biblioteca2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
         <v>237</v>
       </c>
@@ -10553,7 +10552,7 @@
         <v>biblioteca3</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
         <v>238</v>
       </c>
@@ -10568,7 +10567,7 @@
         <v>biblioteca4</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
         <v>239</v>
       </c>
@@ -10583,7 +10582,7 @@
         <v>biblioteca5</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
         <v>240</v>
       </c>
@@ -10614,7 +10613,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14">
       <c r="A43" t="s">
         <v>62</v>
       </c>
@@ -10633,7 +10632,7 @@
         <v>BeigeAzulWengueGrisCaobabiblioteca6Plata</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -10645,62 +10644,62 @@
         <v>biblioteca8</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14">
       <c r="D45" s="1"/>
       <c r="K45" t="str">
         <f t="shared" si="3"/>
         <v>biblioteca9</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14">
       <c r="K46" t="str">
         <f t="shared" si="3"/>
         <v>biblioteca10</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14">
       <c r="K47" t="str">
         <f t="shared" si="3"/>
         <v>biblioteca11</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14">
       <c r="K48" t="str">
         <f t="shared" si="3"/>
         <v>biblioteca12</v>
       </c>
     </row>
-    <row r="49" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="11:11">
       <c r="K49" t="str">
         <f t="shared" si="3"/>
         <v>biblioteca13</v>
       </c>
     </row>
-    <row r="50" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="11:11">
       <c r="K50" t="str">
         <f t="shared" si="3"/>
         <v>biblioteca14</v>
       </c>
     </row>
-    <row r="51" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="11:11">
       <c r="K51" t="str">
         <f t="shared" si="3"/>
         <v>biblioteca15</v>
       </c>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:4">
       <c r="D76" s="1"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:4">
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:4">
       <c r="D78" s="1"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:4">
       <c r="D79" s="1"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7">
       <c r="A100" s="6"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -10709,7 +10708,7 @@
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7">
       <c r="A101" s="1"/>
       <c r="B101" s="2"/>
       <c r="C101" s="1"/>
@@ -10717,7 +10716,7 @@
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -10725,7 +10724,7 @@
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -10733,7 +10732,7 @@
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>

</xml_diff>